<commit_message>
updated checklist with current page numbers and section numbers
</commit_message>
<xml_diff>
--- a/winter/Neo Regression Test Checklist.xlsx
+++ b/winter/Neo Regression Test Checklist.xlsx
@@ -164,30 +164,6 @@
     <t>Automatic Shutdown Sequence (Ice Machine State 5)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Validate that when damper switch is open for more than 30 seconds following </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>harvest cycle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the ice machine will shut down, automatically turning OFF all electrical components.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">During automatic shutdown if the ON/OFF button is pressed for the  Frist Time then the ice machine shall turn OFF and de-energize the ON/OFF LED on the Neo user interface.
 </t>
   </si>
@@ -465,6 +441,9 @@
   </si>
   <si>
     <t>Sub-Section</t>
+  </si>
+  <si>
+    <t>Validate that when damper switch is open for more than 30 seconds following harvest cycle the ice machine will shut down, automatically turning OFF all electrical components.</t>
   </si>
   <si>
     <t>On the second Freeze cycle: connect the pins of the thermistor to a Decade  Box. In pre-chill set resistance value to 22KΩ (45˚F). After entering Freeze, increase resistance the Decade Box to 33KΩ (33˚F). Verify the machine enters the pump pause logic, defined as the water pump de-energizing for25 seconds followed by the water inlet energizing for 7 seconds. Let the freeze cycle complete.</t>
@@ -597,7 +576,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,13 +654,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -789,7 +761,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -907,23 +879,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1264,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1314,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -1360,13 +1329,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>10</v>
@@ -1378,29 +1347,29 @@
         <v>12</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>6.2</v>
+        <v>14</v>
       </c>
       <c r="B9" s="16">
         <v>2</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>13</v>
@@ -1496,7 +1465,7 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>19</v>
@@ -1578,7 +1547,7 @@
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E22" s="16" t="s">
         <v>24</v>
@@ -1940,7 +1909,7 @@
       </c>
       <c r="C48" s="17"/>
       <c r="D48" s="18">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>28</v>
@@ -2083,7 +2052,7 @@
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="25"/>
@@ -2120,7 +2089,7 @@
       </c>
       <c r="C61" s="17"/>
       <c r="D61" s="18">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>39</v>
@@ -2216,7 +2185,7 @@
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="18">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>45</v>
@@ -2233,7 +2202,7 @@
       </c>
       <c r="D69" s="25"/>
       <c r="E69" s="31" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="F69" s="24"/>
       <c r="G69" s="25"/>
@@ -2247,7 +2216,7 @@
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="25"/>
@@ -2261,7 +2230,7 @@
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="25"/>
@@ -2275,7 +2244,7 @@
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="25"/>
@@ -2298,10 +2267,10 @@
       </c>
       <c r="C74" s="17"/>
       <c r="D74" s="18">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F74" s="19"/>
       <c r="G74" s="18"/>
@@ -2315,7 +2284,7 @@
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F75" s="24"/>
       <c r="G75" s="25"/>
@@ -2329,7 +2298,7 @@
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F76" s="24"/>
       <c r="G76" s="25"/>
@@ -2343,7 +2312,7 @@
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F77" s="24"/>
       <c r="G77" s="25"/>
@@ -2357,7 +2326,7 @@
       </c>
       <c r="D78" s="25"/>
       <c r="E78" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F78" s="24"/>
       <c r="G78" s="25"/>
@@ -2371,7 +2340,7 @@
       </c>
       <c r="D79" s="25"/>
       <c r="E79" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F79" s="24"/>
       <c r="G79" s="25"/>
@@ -2385,7 +2354,7 @@
       </c>
       <c r="D80" s="25"/>
       <c r="E80" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F80" s="24"/>
       <c r="G80" s="25"/>
@@ -2399,7 +2368,7 @@
       </c>
       <c r="D81" s="25"/>
       <c r="E81" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F81" s="24"/>
       <c r="G81" s="25"/>
@@ -2413,7 +2382,7 @@
       </c>
       <c r="D82" s="25"/>
       <c r="E82" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F82" s="24"/>
       <c r="G82" s="25"/>
@@ -2427,7 +2396,7 @@
       </c>
       <c r="D83" s="25"/>
       <c r="E83" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="25"/>
@@ -2436,12 +2405,12 @@
     <row r="84" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="33"/>
       <c r="B84" s="20"/>
-      <c r="C84" s="44">
+      <c r="C84" s="43">
         <v>10</v>
       </c>
       <c r="D84" s="25"/>
       <c r="E84" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F84" s="24"/>
       <c r="G84" s="25"/>
@@ -2459,17 +2428,17 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
-        <v>6.3</v>
+        <v>14</v>
       </c>
       <c r="B86" s="16">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C86" s="17"/>
       <c r="D86" s="18">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F86" s="19"/>
       <c r="G86" s="18"/>
@@ -2483,7 +2452,7 @@
       </c>
       <c r="D87" s="25"/>
       <c r="E87" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F87" s="24"/>
       <c r="G87" s="25"/>
@@ -2497,7 +2466,7 @@
       </c>
       <c r="D88" s="25"/>
       <c r="E88" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F88" s="24"/>
       <c r="G88" s="25"/>
@@ -2511,7 +2480,7 @@
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F89" s="24"/>
       <c r="G89" s="25"/>
@@ -2525,7 +2494,7 @@
       </c>
       <c r="D90" s="25"/>
       <c r="E90" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F90" s="24"/>
       <c r="G90" s="25"/>
@@ -2539,7 +2508,7 @@
       </c>
       <c r="D91" s="25"/>
       <c r="E91" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F91" s="24"/>
       <c r="G91" s="25"/>
@@ -2553,7 +2522,7 @@
       </c>
       <c r="D92" s="25"/>
       <c r="E92" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F92" s="24"/>
       <c r="G92" s="25"/>
@@ -2567,7 +2536,7 @@
       </c>
       <c r="D93" s="25"/>
       <c r="E93" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F93" s="24"/>
       <c r="G93" s="25"/>
@@ -2581,7 +2550,7 @@
       </c>
       <c r="D94" s="25"/>
       <c r="E94" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F94" s="24"/>
       <c r="G94" s="25"/>
@@ -2595,7 +2564,7 @@
       </c>
       <c r="D95" s="25"/>
       <c r="E95" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F95" s="24"/>
       <c r="G95" s="25"/>
@@ -2609,7 +2578,7 @@
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F96" s="24"/>
       <c r="G96" s="25"/>
@@ -2623,7 +2592,7 @@
       </c>
       <c r="D97" s="25"/>
       <c r="E97" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F97" s="24"/>
       <c r="G97" s="25"/>
@@ -2637,7 +2606,7 @@
       </c>
       <c r="D98" s="25"/>
       <c r="E98" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F98" s="24"/>
       <c r="G98" s="25"/>
@@ -2651,7 +2620,7 @@
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F99" s="24"/>
       <c r="G99" s="25"/>
@@ -2665,7 +2634,7 @@
       </c>
       <c r="D100" s="25"/>
       <c r="E100" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F100" s="24"/>
       <c r="G100" s="25"/>
@@ -2679,7 +2648,7 @@
       </c>
       <c r="D101" s="25"/>
       <c r="E101" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F101" s="24"/>
       <c r="G101" s="25"/>
@@ -2693,7 +2662,7 @@
       </c>
       <c r="D102" s="25"/>
       <c r="E102" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F102" s="24"/>
       <c r="G102" s="25"/>
@@ -2707,7 +2676,7 @@
       </c>
       <c r="D103" s="25"/>
       <c r="E103" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F103" s="24"/>
       <c r="G103" s="25"/>
@@ -2721,7 +2690,7 @@
       </c>
       <c r="D104" s="25"/>
       <c r="E104" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F104" s="24"/>
       <c r="G104" s="25"/>
@@ -2735,7 +2704,7 @@
       </c>
       <c r="D105" s="25"/>
       <c r="E105" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F105" s="24"/>
       <c r="G105" s="25"/>
@@ -2749,7 +2718,7 @@
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F106" s="24"/>
       <c r="G106" s="25"/>
@@ -2776,16 +2745,18 @@
       <c r="H108" s="28"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="45">
-        <v>6.4</v>
-      </c>
-      <c r="B109" s="40"/>
+      <c r="A109" s="44">
+        <v>14</v>
+      </c>
+      <c r="B109" s="44">
+        <v>10</v>
+      </c>
       <c r="C109" s="17"/>
       <c r="D109" s="18">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F109" s="19"/>
       <c r="G109" s="18"/>
@@ -2799,7 +2770,7 @@
       </c>
       <c r="D110" s="25"/>
       <c r="E110" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F110" s="24"/>
       <c r="G110" s="25"/>
@@ -2813,7 +2784,7 @@
       </c>
       <c r="D111" s="25"/>
       <c r="E111" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F111" s="24"/>
       <c r="G111" s="25"/>
@@ -2827,7 +2798,7 @@
       </c>
       <c r="D112" s="25"/>
       <c r="E112" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F112" s="24"/>
       <c r="G112" s="25"/>
@@ -2841,7 +2812,7 @@
       </c>
       <c r="D113" s="25"/>
       <c r="E113" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F113" s="24"/>
       <c r="G113" s="25"/>
@@ -2859,17 +2830,17 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="16">
-        <v>6.5</v>
+        <v>14</v>
       </c>
       <c r="B115" s="16">
-        <v>1</v>
+        <v>11.1</v>
       </c>
       <c r="C115" s="17"/>
       <c r="D115" s="18">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F115" s="19"/>
       <c r="G115" s="18"/>
@@ -2883,7 +2854,7 @@
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F116" s="24"/>
       <c r="G116" s="25"/>
@@ -2897,7 +2868,7 @@
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F117" s="24"/>
       <c r="G117" s="25"/>
@@ -2911,7 +2882,7 @@
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F118" s="24"/>
       <c r="G118" s="25"/>
@@ -2925,7 +2896,7 @@
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F119" s="24"/>
       <c r="G119" s="25"/>
@@ -2939,7 +2910,7 @@
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F120" s="24"/>
       <c r="G120" s="25"/>
@@ -2948,7 +2919,7 @@
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="34"/>
       <c r="B121" s="34"/>
-      <c r="C121" s="41"/>
+      <c r="C121" s="40"/>
       <c r="D121" s="28"/>
       <c r="E121" s="39"/>
       <c r="F121" s="24"/>
@@ -2958,14 +2929,14 @@
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="16"/>
       <c r="B122" s="16">
-        <v>2</v>
+        <v>11.2</v>
       </c>
       <c r="C122" s="17"/>
       <c r="D122" s="18">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E122" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F122" s="19"/>
       <c r="G122" s="18"/>
@@ -2979,7 +2950,7 @@
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F123" s="24"/>
       <c r="G123" s="25"/>
@@ -2993,7 +2964,7 @@
       </c>
       <c r="D124" s="25"/>
       <c r="E124" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F124" s="24"/>
       <c r="G124" s="25"/>
@@ -3007,7 +2978,7 @@
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F125" s="24"/>
       <c r="G125" s="25"/>
@@ -3021,7 +2992,7 @@
       </c>
       <c r="D126" s="25"/>
       <c r="E126" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F126" s="24"/>
       <c r="G126" s="25"/>
@@ -3035,7 +3006,7 @@
       </c>
       <c r="D127" s="25"/>
       <c r="E127" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F127" s="24"/>
       <c r="G127" s="25"/>
@@ -3049,7 +3020,7 @@
       </c>
       <c r="D128" s="25"/>
       <c r="E128" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F128" s="24"/>
       <c r="G128" s="25"/>
@@ -3068,14 +3039,14 @@
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="16"/>
       <c r="B130" s="16">
-        <v>3</v>
+        <v>11.3</v>
       </c>
       <c r="C130" s="17"/>
       <c r="D130" s="18">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E130" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F130" s="19"/>
       <c r="G130" s="18"/>
@@ -3089,7 +3060,7 @@
       </c>
       <c r="D131" s="25"/>
       <c r="E131" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F131" s="24"/>
       <c r="G131" s="25"/>
@@ -3103,7 +3074,7 @@
       </c>
       <c r="D132" s="25"/>
       <c r="E132" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F132" s="24"/>
       <c r="G132" s="25"/>
@@ -3117,7 +3088,7 @@
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F133" s="24"/>
       <c r="G133" s="25"/>
@@ -3131,7 +3102,7 @@
       </c>
       <c r="D134" s="25"/>
       <c r="E134" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F134" s="24"/>
       <c r="G134" s="25"/>
@@ -3145,7 +3116,7 @@
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F135" s="24"/>
       <c r="G135" s="25"/>
@@ -3159,7 +3130,7 @@
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F136" s="24"/>
       <c r="G136" s="25"/>
@@ -3173,7 +3144,7 @@
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F137" s="24"/>
       <c r="G137" s="25"/>
@@ -3187,7 +3158,7 @@
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F138" s="24"/>
       <c r="G138" s="25"/>
@@ -3201,7 +3172,7 @@
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F139" s="24"/>
       <c r="G139" s="25"/>
@@ -3215,7 +3186,7 @@
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F140" s="24"/>
       <c r="G140" s="25"/>
@@ -3229,7 +3200,7 @@
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F141" s="24"/>
       <c r="G141" s="25"/>
@@ -3247,15 +3218,17 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="16">
-        <v>6.6</v>
-      </c>
-      <c r="B143" s="16"/>
+        <v>14</v>
+      </c>
+      <c r="B143" s="16">
+        <v>12</v>
+      </c>
       <c r="C143" s="17"/>
       <c r="D143" s="18">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E143" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F143" s="19"/>
       <c r="G143" s="18"/>
@@ -3269,7 +3242,7 @@
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F144" s="25"/>
       <c r="G144" s="25"/>
@@ -3283,7 +3256,7 @@
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F145" s="25"/>
       <c r="G145" s="25"/>
@@ -3297,7 +3270,7 @@
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F146" s="25"/>
       <c r="G146" s="25"/>
@@ -3311,7 +3284,7 @@
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F147" s="25"/>
       <c r="G147" s="25"/>
@@ -3325,7 +3298,7 @@
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F148" s="25"/>
       <c r="G148" s="25"/>
@@ -3339,7 +3312,7 @@
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F149" s="25"/>
       <c r="G149" s="25"/>
@@ -3353,7 +3326,7 @@
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F150" s="25"/>
       <c r="G150" s="25"/>
@@ -3367,7 +3340,7 @@
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F151" s="25"/>
       <c r="G151" s="25"/>
@@ -3381,7 +3354,7 @@
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F152" s="25"/>
       <c r="G152" s="25"/>
@@ -3395,38 +3368,38 @@
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F153" s="25"/>
       <c r="G153" s="25"/>
       <c r="H153" s="25"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A154" s="42"/>
-      <c r="B154" s="42"/>
-      <c r="C154" s="42"/>
+      <c r="A154" s="41"/>
+      <c r="B154" s="41"/>
+      <c r="C154" s="41"/>
       <c r="D154" s="28"/>
-      <c r="E154" s="43"/>
+      <c r="E154" s="42"/>
       <c r="F154" s="28"/>
       <c r="G154" s="30"/>
       <c r="H154" s="28"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="42"/>
-      <c r="B155" s="42"/>
-      <c r="C155" s="42"/>
+      <c r="A155" s="41"/>
+      <c r="B155" s="41"/>
+      <c r="C155" s="41"/>
       <c r="D155" s="28"/>
-      <c r="E155" s="43"/>
+      <c r="E155" s="42"/>
       <c r="F155" s="28"/>
       <c r="G155" s="30"/>
       <c r="H155" s="28"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="42"/>
-      <c r="B156" s="42"/>
-      <c r="C156" s="42"/>
+      <c r="A156" s="41"/>
+      <c r="B156" s="41"/>
+      <c r="C156" s="41"/>
       <c r="D156" s="28"/>
-      <c r="E156" s="43"/>
+      <c r="E156" s="42"/>
       <c r="F156" s="28"/>
       <c r="G156" s="30"/>
       <c r="H156" s="28"/>

</xml_diff>